<commit_message>
Validaciones en CRU's y registros.
Se agregan validaciones respectivas al tamaño de los campos en base de
datos y se aplicó la función trim en todos los CRU's y registros.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C062B9-CFF2-47C4-973C-6C0B5CF40530}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7D706E-9D2B-4BEE-A9FD-DEA45D1BDC8D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,12 +432,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -464,6 +458,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,10 +772,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,84 +850,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="25"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="16"/>
+      <c r="L4" s="25"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="16"/>
+      <c r="O4" s="25"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="16"/>
+      <c r="R4" s="25"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="16"/>
+      <c r="U4" s="25"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="15" t="s">
+      <c r="W4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="16"/>
+      <c r="X4" s="25"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="15" t="s">
+      <c r="Z4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="16"/>
+      <c r="AA4" s="25"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="15" t="s">
+      <c r="AC4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="16"/>
+      <c r="AD4" s="25"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="15" t="s">
+      <c r="AF4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="16"/>
+      <c r="AG4" s="25"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="15" t="s">
+      <c r="AI4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="16"/>
+      <c r="AJ4" s="25"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="15" t="s">
+      <c r="AL4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="16"/>
+      <c r="AM4" s="25"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="15" t="s">
+      <c r="AO4" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="16"/>
+      <c r="AP4" s="25"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="15" t="s">
+      <c r="AR4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="16"/>
+      <c r="AS4" s="25"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="15" t="s">
+      <c r="AU4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="16"/>
+      <c r="AV4" s="25"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="15" t="s">
+      <c r="AX4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="16"/>
-      <c r="AZ4" s="15" t="s">
+      <c r="AY4" s="25"/>
+      <c r="AZ4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="16"/>
+      <c r="BA4" s="25"/>
     </row>
     <row r="5" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1062,10 +1062,10 @@
     <row r="6" spans="2:53" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="18" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1074,111 +1074,113 @@
       <c r="G6" s="5">
         <v>4</v>
       </c>
-      <c r="H6" s="8"/>
+      <c r="H6" s="8">
+        <v>2</v>
+      </c>
       <c r="I6" s="8">
         <f>G6-H6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8">
         <f t="shared" ref="L6:L16" si="0">I6-K6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8">
         <f t="shared" ref="O6:O16" si="1">L6-N6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8">
         <f t="shared" ref="R6:R16" si="2">O6-Q6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S6" s="10"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8">
         <f t="shared" ref="U6:U16" si="3">R6-T6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" ref="X6:X16" si="4">U6-W6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
         <f t="shared" ref="AA6:AA16" si="5">X6-Z6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
         <f t="shared" ref="AD6:AD16" si="6">AA6-AC6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
         <f t="shared" ref="AG6:AG16" si="7">AD6-AF6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
         <f t="shared" ref="AJ6:AJ16" si="8">AG6-AI6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
         <f t="shared" ref="AM6:AM16" si="9">AJ6-AL6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
         <f t="shared" ref="AP6:AP16" si="10">AM6-AO6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
         <f t="shared" ref="AS6:AS16" si="11">AP6-AR6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
         <f t="shared" ref="AV6:AV16" si="12">AS6-AU6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
         <f t="shared" ref="AY6:AY16" si="13">AV6-AX6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AZ6" s="11">
         <f t="shared" ref="AZ6:AZ16" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA16" si="15">G6-AZ6</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:53" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="19" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -1288,10 +1290,10 @@
     <row r="8" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="19" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -1401,10 +1403,10 @@
     <row r="9" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="18" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1514,10 +1516,10 @@
     <row r="10" spans="2:53" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="19" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1630,7 +1632,7 @@
       <c r="D11" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="19" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -1740,10 +1742,10 @@
     <row r="12" spans="2:53" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="18" t="s">
         <v>42</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1853,10 +1855,10 @@
     <row r="13" spans="2:53" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="18" t="s">
         <v>42</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -1966,10 +1968,10 @@
     <row r="14" spans="2:53" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="24" t="s">
+      <c r="D14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="19" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -2079,10 +2081,10 @@
     <row r="15" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="18" t="s">
         <v>42</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -2193,7 +2195,7 @@
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="17"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="8"/>
@@ -2610,6 +2612,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2621,11 +2628,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correcciones de la entrega 40%
Se muestra la lista de pagos de alumnos en orden inverso asi como solo los profesores activos.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7D706E-9D2B-4BEE-A9FD-DEA45D1BDC8D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8A62927F-B2E8-4ABF-8A93-99A424AD67EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -195,8 +195,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +229,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -398,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -465,12 +473,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{7D707B13-ED15-43BF-9B27-CEF53E2D3B45}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -775,7 +814,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,102 +1228,104 @@
       <c r="G7" s="5">
         <v>2</v>
       </c>
-      <c r="H7" s="8"/>
+      <c r="H7" s="8">
+        <v>2</v>
+      </c>
       <c r="I7" s="8">
         <f t="shared" ref="I7:I16" si="16">G7-H7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="8"/>
       <c r="O7" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S7" s="10"/>
       <c r="T7" s="8"/>
       <c r="U7" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:53" ht="45" x14ac:dyDescent="0.25">
@@ -1296,108 +1337,110 @@
       <c r="E8" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="26" t="s">
         <v>41</v>
       </c>
       <c r="G8" s="5">
         <v>2</v>
       </c>
-      <c r="H8" s="8"/>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
       <c r="I8" s="8">
         <f t="shared" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="8"/>
       <c r="O8" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P8" s="10"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S8" s="10"/>
       <c r="T8" s="8"/>
       <c r="U8" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB8" s="10"/>
       <c r="AC8" s="8"/>
       <c r="AD8" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="8"/>
       <c r="AG8" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH8" s="10"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK8" s="10"/>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN8" s="10"/>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="8"/>
       <c r="AS8" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT8" s="10"/>
       <c r="AU8" s="8"/>
       <c r="AV8" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW8" s="10"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:53" ht="45" x14ac:dyDescent="0.25">
@@ -2612,11 +2655,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2628,6 +2666,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Alumnos en orden alfabético
Los alumnos de los catalogos y la vista por grupo aparecen en orden
alfabético. Se actualiza la plantilla de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8A62927F-B2E8-4ABF-8A93-99A424AD67EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590BC4A4-F34C-4DEC-A453-810FCF93E0CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
   <si>
     <t>Columna</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>CU 08 - Inscribir alumno.</t>
+  </si>
+  <si>
+    <t>Hecho</t>
   </si>
 </sst>
 </file>
@@ -467,14 +470,14 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -811,10 +814,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,84 +892,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="25"/>
+      <c r="I4" s="26"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="25"/>
+      <c r="L4" s="26"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="25"/>
+      <c r="O4" s="26"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="25"/>
+      <c r="R4" s="26"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="24" t="s">
+      <c r="T4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="25"/>
+      <c r="U4" s="26"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="24" t="s">
+      <c r="W4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="25"/>
+      <c r="X4" s="26"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="24" t="s">
+      <c r="Z4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="25"/>
+      <c r="AA4" s="26"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="24" t="s">
+      <c r="AC4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="25"/>
+      <c r="AD4" s="26"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="24" t="s">
+      <c r="AF4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="25"/>
+      <c r="AG4" s="26"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="24" t="s">
+      <c r="AI4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="25"/>
+      <c r="AJ4" s="26"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="24" t="s">
+      <c r="AL4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="25"/>
+      <c r="AM4" s="26"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="24" t="s">
+      <c r="AO4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="25"/>
+      <c r="AP4" s="26"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="24" t="s">
+      <c r="AR4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="25"/>
+      <c r="AS4" s="26"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="24" t="s">
+      <c r="AU4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="25"/>
+      <c r="AV4" s="26"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="24" t="s">
+      <c r="AX4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="25"/>
-      <c r="AZ4" s="24" t="s">
+      <c r="AY4" s="26"/>
+      <c r="AZ4" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="25"/>
+      <c r="BA4" s="26"/>
     </row>
     <row r="5" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1108,7 +1111,7 @@
         <v>42</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G6" s="5">
         <v>4</v>
@@ -1223,7 +1226,7 @@
         <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G7" s="5">
         <v>2</v>
@@ -1337,8 +1340,8 @@
       <c r="E8" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="26" t="s">
-        <v>41</v>
+      <c r="F8" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="G8" s="5">
         <v>2</v>
@@ -1453,7 +1456,7 @@
         <v>42</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G9" s="5">
         <v>4</v>
@@ -1464,96 +1467,98 @@
         <v>4</v>
       </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="8"/>
+      <c r="K9" s="8">
+        <v>3</v>
+      </c>
       <c r="L9" s="8">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="S9" s="10"/>
       <c r="T9" s="8"/>
       <c r="U9" s="8">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="8"/>
       <c r="X9" s="8">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="10"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AB9" s="10"/>
       <c r="AC9" s="8"/>
       <c r="AD9" s="8">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AE9" s="10"/>
       <c r="AF9" s="8"/>
       <c r="AG9" s="8">
         <f t="shared" si="7"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AH9" s="10"/>
       <c r="AI9" s="8"/>
       <c r="AJ9" s="8">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AK9" s="10"/>
       <c r="AL9" s="8"/>
       <c r="AM9" s="8">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AN9" s="10"/>
       <c r="AO9" s="8"/>
       <c r="AP9" s="8">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AQ9" s="10"/>
       <c r="AR9" s="8"/>
       <c r="AS9" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AT9" s="10"/>
       <c r="AU9" s="8"/>
       <c r="AV9" s="8">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AW9" s="10"/>
       <c r="AX9" s="8"/>
       <c r="AY9" s="8">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AZ9" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BA9" s="11">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:53" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2655,6 +2660,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2666,11 +2676,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mecanismo para obtener fotos de alumnos.
Se implementa el mecanismo deobtención de fotos del sistema para los usuarios del sistema.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590BC4A4-F34C-4DEC-A453-810FCF93E0CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A1929C17-89A7-44FE-A32E-B2665FD62D18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -440,9 +440,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -478,6 +475,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,10 +814,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,84 +892,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="26"/>
+      <c r="I4" s="25"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="26"/>
+      <c r="L4" s="25"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="26"/>
+      <c r="O4" s="25"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="25" t="s">
+      <c r="Q4" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="26"/>
+      <c r="R4" s="25"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="26"/>
+      <c r="U4" s="25"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="25" t="s">
+      <c r="W4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="26"/>
+      <c r="X4" s="25"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="25" t="s">
+      <c r="Z4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="26"/>
+      <c r="AA4" s="25"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="25" t="s">
+      <c r="AC4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="26"/>
+      <c r="AD4" s="25"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="25" t="s">
+      <c r="AF4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="26"/>
+      <c r="AG4" s="25"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="25" t="s">
+      <c r="AI4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="26"/>
+      <c r="AJ4" s="25"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="25" t="s">
+      <c r="AL4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="26"/>
+      <c r="AM4" s="25"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="25" t="s">
+      <c r="AO4" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="26"/>
+      <c r="AP4" s="25"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="25" t="s">
+      <c r="AR4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="26"/>
+      <c r="AS4" s="25"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="25" t="s">
+      <c r="AU4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="26"/>
+      <c r="AV4" s="25"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="25" t="s">
+      <c r="AX4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="26"/>
-      <c r="AZ4" s="25" t="s">
+      <c r="AY4" s="25"/>
+      <c r="AZ4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="26"/>
+      <c r="BA4" s="25"/>
     </row>
     <row r="5" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1104,10 +1104,10 @@
     <row r="6" spans="2:53" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1219,10 +1219,10 @@
     <row r="7" spans="2:53" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -1334,13 +1334,13 @@
     <row r="8" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="23" t="s">
         <v>53</v>
       </c>
       <c r="G8" s="5">
@@ -1449,10 +1449,10 @@
     <row r="9" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -1564,10 +1564,10 @@
     <row r="10" spans="2:53" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1588,99 +1588,101 @@
         <v>2</v>
       </c>
       <c r="M10" s="10"/>
-      <c r="N10" s="8"/>
+      <c r="N10" s="8">
+        <v>2</v>
+      </c>
       <c r="O10" s="8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S10" s="10"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="8"/>
       <c r="X10" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y10" s="10"/>
       <c r="Z10" s="8"/>
       <c r="AA10" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB10" s="10"/>
       <c r="AC10" s="8"/>
       <c r="AD10" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE10" s="10"/>
       <c r="AF10" s="8"/>
       <c r="AG10" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH10" s="10"/>
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK10" s="10"/>
       <c r="AL10" s="8"/>
       <c r="AM10" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN10" s="10"/>
       <c r="AO10" s="8"/>
       <c r="AP10" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="8"/>
       <c r="AS10" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT10" s="10"/>
       <c r="AU10" s="8"/>
       <c r="AV10" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW10" s="10"/>
       <c r="AX10" s="8"/>
       <c r="AY10" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ10" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA10" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:53" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
@@ -1790,10 +1792,10 @@
     <row r="12" spans="2:53" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1903,10 +1905,10 @@
     <row r="13" spans="2:53" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -2016,10 +2018,10 @@
     <row r="14" spans="2:53" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -2129,10 +2131,10 @@
     <row r="15" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="17" t="s">
         <v>42</v>
       </c>
       <c r="F15" s="5" t="s">
@@ -2243,7 +2245,7 @@
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="15"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="8"/>
@@ -2660,11 +2662,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2676,6 +2673,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajuste de paneles en listas
Se ajustan los paneles de todas las listas para abarcar todo el ancho
disponible.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{A1929C17-89A7-44FE-A32E-B2665FD62D18}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6A2B9A-BE95-4611-8D6B-0E65CF1F3F63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
   <si>
     <t>Columna</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Hecho</t>
+  </si>
+  <si>
+    <t>En proceso</t>
   </si>
 </sst>
 </file>
@@ -470,14 +473,14 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,10 +817,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,84 +895,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="25"/>
+      <c r="I4" s="26"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="25"/>
+      <c r="L4" s="26"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="24" t="s">
+      <c r="N4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="25"/>
+      <c r="O4" s="26"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="25"/>
+      <c r="R4" s="26"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="24" t="s">
+      <c r="T4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="25"/>
+      <c r="U4" s="26"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="24" t="s">
+      <c r="W4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="25"/>
+      <c r="X4" s="26"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="24" t="s">
+      <c r="Z4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="25"/>
+      <c r="AA4" s="26"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="24" t="s">
+      <c r="AC4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="25"/>
+      <c r="AD4" s="26"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="24" t="s">
+      <c r="AF4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="25"/>
+      <c r="AG4" s="26"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="24" t="s">
+      <c r="AI4" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="25"/>
+      <c r="AJ4" s="26"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="24" t="s">
+      <c r="AL4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="25"/>
+      <c r="AM4" s="26"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="24" t="s">
+      <c r="AO4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="25"/>
+      <c r="AP4" s="26"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="24" t="s">
+      <c r="AR4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="25"/>
+      <c r="AS4" s="26"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="24" t="s">
+      <c r="AU4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="25"/>
+      <c r="AV4" s="26"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="24" t="s">
+      <c r="AX4" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="25"/>
-      <c r="AZ4" s="24" t="s">
+      <c r="AY4" s="26"/>
+      <c r="AZ4" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="25"/>
+      <c r="BA4" s="26"/>
     </row>
     <row r="5" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1571,7 +1574,7 @@
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="G10" s="5">
         <v>2</v>
@@ -1679,7 +1682,7 @@
     <row r="11" spans="2:53" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="24" t="s">
         <v>50</v>
       </c>
       <c r="E11" s="18" t="s">
@@ -1799,7 +1802,7 @@
         <v>42</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="G12" s="5">
         <v>2</v>
@@ -1816,90 +1819,92 @@
         <v>2</v>
       </c>
       <c r="M12" s="10"/>
-      <c r="N12" s="8"/>
+      <c r="N12" s="8">
+        <v>2</v>
+      </c>
       <c r="O12" s="8">
         <f>L12-N12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8">
         <f>O12-Q12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S12" s="10"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8">
         <f>R12-T12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V12" s="10"/>
       <c r="W12" s="8"/>
       <c r="X12" s="8">
         <f>U12-W12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="10"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8">
         <f>X12-Z12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB12" s="10"/>
       <c r="AC12" s="8"/>
       <c r="AD12" s="8">
         <f>AA12-AC12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AE12" s="10"/>
       <c r="AF12" s="8"/>
       <c r="AG12" s="8">
         <f>AD12-AF12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH12" s="10"/>
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8">
         <f>AG12-AI12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK12" s="10"/>
       <c r="AL12" s="8"/>
       <c r="AM12" s="8">
         <f>AJ12-AL12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN12" s="10"/>
       <c r="AO12" s="8"/>
       <c r="AP12" s="8">
         <f>AM12-AO12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="8"/>
       <c r="AS12" s="8">
         <f>AP12-AR12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT12" s="10"/>
       <c r="AU12" s="8"/>
       <c r="AV12" s="8">
         <f>AS12-AU12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW12" s="10"/>
       <c r="AX12" s="8"/>
       <c r="AY12" s="8">
         <f>AV12-AX12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ12" s="11">
         <f>H12+K12+N12+Q12+T12+W12+Z12+AC12+AF12+AI12+AL12+AO12+AR12+AU12+AX12</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA12" s="11">
         <f>G12-AZ12</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:53" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2662,6 +2667,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2673,11 +2683,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Nombre de grupo & fecha de inicio en profesor
Se aumenta el espacio de visualización para el nombre de grupo, se
implementa en interfaz un DatePicker para seleccionar la fecha de inicio
de pago, se agrega en logica el campo fechaInicio, se agrega espacio
para imágen de cliente, se hacen modificaciones menores a dimensiones de
interfáz y se actualizan plantillas de tareas y casos de uso.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6A2B9A-BE95-4611-8D6B-0E65CF1F3F63}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F275D091-CAEE-451F-BBAE-C5042DB693DF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -817,10 +817,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,7 +1802,7 @@
         <v>42</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="5">
         <v>2</v>
@@ -1827,84 +1827,86 @@
         <v>0</v>
       </c>
       <c r="P12" s="10"/>
-      <c r="Q12" s="8"/>
+      <c r="Q12" s="8">
+        <v>1</v>
+      </c>
       <c r="R12" s="8">
         <f>O12-Q12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S12" s="10"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8">
         <f>R12-T12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="V12" s="10"/>
       <c r="W12" s="8"/>
       <c r="X12" s="8">
         <f>U12-W12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y12" s="10"/>
       <c r="Z12" s="8"/>
       <c r="AA12" s="8">
         <f>X12-Z12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB12" s="10"/>
       <c r="AC12" s="8"/>
       <c r="AD12" s="8">
         <f>AA12-AC12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE12" s="10"/>
       <c r="AF12" s="8"/>
       <c r="AG12" s="8">
         <f>AD12-AF12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AH12" s="10"/>
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8">
         <f>AG12-AI12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK12" s="10"/>
       <c r="AL12" s="8"/>
       <c r="AM12" s="8">
         <f>AJ12-AL12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN12" s="10"/>
       <c r="AO12" s="8"/>
       <c r="AP12" s="8">
         <f>AM12-AO12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="8"/>
       <c r="AS12" s="8">
         <f>AP12-AR12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT12" s="10"/>
       <c r="AU12" s="8"/>
       <c r="AV12" s="8">
         <f>AS12-AU12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW12" s="10"/>
       <c r="AX12" s="8"/>
       <c r="AY12" s="8">
         <f>AV12-AX12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ12" s="11">
         <f>H12+K12+N12+Q12+T12+W12+Z12+AC12+AF12+AI12+AL12+AO12+AR12+AU12+AX12</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BA12" s="11">
         <f>G12-AZ12</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="13" spans="2:53" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1917,7 +1919,7 @@
         <v>42</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="G13" s="5">
         <v>3</v>
@@ -1940,84 +1942,86 @@
         <v>3</v>
       </c>
       <c r="P13" s="10"/>
-      <c r="Q13" s="8"/>
+      <c r="Q13" s="8">
+        <v>1</v>
+      </c>
       <c r="R13" s="8">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S13" s="10"/>
       <c r="T13" s="8"/>
       <c r="U13" s="8">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V13" s="10"/>
       <c r="W13" s="8"/>
       <c r="X13" s="8">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB13" s="10"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE13" s="10"/>
       <c r="AF13" s="8"/>
       <c r="AG13" s="8">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH13" s="10"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK13" s="10"/>
       <c r="AL13" s="8"/>
       <c r="AM13" s="8">
         <f t="shared" si="9"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AN13" s="10"/>
       <c r="AO13" s="8"/>
       <c r="AP13" s="8">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="8">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AT13" s="10"/>
       <c r="AU13" s="8"/>
       <c r="AV13" s="8">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AW13" s="10"/>
       <c r="AX13" s="8"/>
       <c r="AY13" s="8">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AZ13" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA13" s="11">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:53" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2667,11 +2671,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2683,6 +2682,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mecanismo para obtener fotos.
Se implementa el mecanismo para obtener fotos de los usuarios desde
alguna ruta del sistema.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
-  <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F275D091-CAEE-451F-BBAE-C5042DB693DF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -201,7 +195,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -511,7 +505,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{7D707B13-ED15-43BF-9B27-CEF53E2D3B45}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -813,14 +807,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="R13" sqref="R13"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,10 +1579,12 @@
         <v>2</v>
       </c>
       <c r="J10" s="10"/>
-      <c r="K10" s="8"/>
+      <c r="K10" s="8">
+        <v>3</v>
+      </c>
       <c r="L10" s="8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="8">
@@ -1596,87 +1592,87 @@
       </c>
       <c r="O10" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="S10" s="10"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="8"/>
       <c r="X10" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="Y10" s="10"/>
       <c r="Z10" s="8"/>
       <c r="AA10" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AB10" s="10"/>
       <c r="AC10" s="8"/>
       <c r="AD10" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AE10" s="10"/>
       <c r="AF10" s="8"/>
       <c r="AG10" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AH10" s="10"/>
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AK10" s="10"/>
       <c r="AL10" s="8"/>
       <c r="AM10" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AN10" s="10"/>
       <c r="AO10" s="8"/>
       <c r="AP10" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="8"/>
       <c r="AS10" s="8">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AT10" s="10"/>
       <c r="AU10" s="8"/>
       <c r="AV10" s="8">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AW10" s="10"/>
       <c r="AX10" s="8"/>
       <c r="AY10" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="AZ10" s="11">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="BA10" s="11">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="11" spans="2:53" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -2671,6 +2667,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2682,11 +2683,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2704,7 +2700,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Fecha de inicio de pago
Se agrega completamente el campo fechaInicio a la entidad Profesor, se
actuañlizan plantillas de casos de uso y lista de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE39DF3C-A9FC-404C-8109-6043C41A9C6D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -195,7 +201,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -505,7 +511,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -564,7 +570,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -597,9 +603,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -632,6 +655,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -807,14 +847,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,78 +1986,80 @@
         <v>2</v>
       </c>
       <c r="S13" s="10"/>
-      <c r="T13" s="8"/>
+      <c r="T13" s="8">
+        <v>1</v>
+      </c>
       <c r="U13" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V13" s="10"/>
       <c r="W13" s="8"/>
       <c r="X13" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB13" s="10"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE13" s="10"/>
       <c r="AF13" s="8"/>
       <c r="AG13" s="8">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH13" s="10"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK13" s="10"/>
       <c r="AL13" s="8"/>
       <c r="AM13" s="8">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN13" s="10"/>
       <c r="AO13" s="8"/>
       <c r="AP13" s="8">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="8">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT13" s="10"/>
       <c r="AU13" s="8"/>
       <c r="AV13" s="8">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AW13" s="10"/>
       <c r="AX13" s="8"/>
       <c r="AY13" s="8">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ13" s="11">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BA13" s="11">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:53" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2667,11 +2709,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2683,6 +2720,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2700,7 +2742,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Mecanismo de amacenamiento de imagenes,
Se implementa el mecanismo  de almacenamiento de images en el proyecto.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE39DF3C-A9FC-404C-8109-6043C41A9C6D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2DC7C87A-91F8-4292-9127-8CD08A3CA963}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -851,10 +851,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="W13" sqref="W13"/>
+      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,84 +1635,86 @@
         <v>-3</v>
       </c>
       <c r="P10" s="10"/>
-      <c r="Q10" s="8"/>
+      <c r="Q10" s="8">
+        <v>1</v>
+      </c>
       <c r="R10" s="8">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="S10" s="10"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8">
         <f t="shared" si="3"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="V10" s="10"/>
       <c r="W10" s="8"/>
       <c r="X10" s="8">
         <f t="shared" si="4"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="Y10" s="10"/>
       <c r="Z10" s="8"/>
       <c r="AA10" s="8">
         <f t="shared" si="5"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AB10" s="10"/>
       <c r="AC10" s="8"/>
       <c r="AD10" s="8">
         <f t="shared" si="6"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AE10" s="10"/>
       <c r="AF10" s="8"/>
       <c r="AG10" s="8">
         <f t="shared" si="7"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AH10" s="10"/>
       <c r="AI10" s="8"/>
       <c r="AJ10" s="8">
         <f t="shared" si="8"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AK10" s="10"/>
       <c r="AL10" s="8"/>
       <c r="AM10" s="8">
         <f t="shared" si="9"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AN10" s="10"/>
       <c r="AO10" s="8"/>
       <c r="AP10" s="8">
         <f t="shared" si="10"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="8"/>
       <c r="AS10" s="8">
         <f t="shared" si="11"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AT10" s="10"/>
       <c r="AU10" s="8"/>
       <c r="AV10" s="8">
         <f t="shared" si="12"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AW10" s="10"/>
       <c r="AX10" s="8"/>
       <c r="AY10" s="8">
         <f t="shared" si="13"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AZ10" s="11">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="BA10" s="11">
         <f t="shared" si="15"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="11" spans="2:53" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -2709,6 +2711,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2720,11 +2727,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Consulta de alumnos activos.
Se corrige en grupos de profesor que solo se puedan mostrar los alumnos activos en ese grupo.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2DC7C87A-91F8-4292-9127-8CD08A3CA963}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6B0093B1-4658-493A-9D21-5D91A064DFB2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -854,7 +854,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomRight" activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1608,7 @@
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" s="5">
         <v>2</v>
@@ -1727,7 +1727,7 @@
         <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G11" s="5">
         <v>1</v>
@@ -1756,78 +1756,80 @@
         <v>1</v>
       </c>
       <c r="S11" s="10"/>
-      <c r="T11" s="8"/>
+      <c r="T11" s="8">
+        <v>1</v>
+      </c>
       <c r="U11" s="8">
         <f>R11-T11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V11" s="10"/>
       <c r="W11" s="8"/>
       <c r="X11" s="8">
         <f>U11-W11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y11" s="10"/>
       <c r="Z11" s="8"/>
       <c r="AA11" s="8">
         <f>X11-Z11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB11" s="10"/>
       <c r="AC11" s="8"/>
       <c r="AD11" s="8">
         <f>AA11-AC11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE11" s="10"/>
       <c r="AF11" s="8"/>
       <c r="AG11" s="8">
         <f>AD11-AF11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH11" s="10"/>
       <c r="AI11" s="8"/>
       <c r="AJ11" s="8">
         <f>AG11-AI11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK11" s="10"/>
       <c r="AL11" s="8"/>
       <c r="AM11" s="8">
         <f>AJ11-AL11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN11" s="10"/>
       <c r="AO11" s="8"/>
       <c r="AP11" s="8">
         <f>AM11-AO11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ11" s="10"/>
       <c r="AR11" s="8"/>
       <c r="AS11" s="8">
         <f>AP11-AR11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT11" s="10"/>
       <c r="AU11" s="8"/>
       <c r="AV11" s="8">
         <f>AS11-AU11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW11" s="10"/>
       <c r="AX11" s="8"/>
       <c r="AY11" s="8">
         <f>AV11-AX11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ11" s="11">
         <f>H11+K11+N11+Q11+T11+W11+Z11+AC11+AF11+AI11+AL11+AO11+AR11+AU11+AX11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA11" s="11">
         <f>G11-AZ11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:53" ht="75" x14ac:dyDescent="0.25">
@@ -2711,11 +2713,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2727,6 +2724,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Profesor en gasto promocional.
Se vincula un profesor con un gasto promocional.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2DC7C87A-91F8-4292-9127-8CD08A3CA963}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7972FB12-94F5-4258-85AC-F6988FC8CC17}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -851,10 +851,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomRight" activeCell="W14" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,7 +1608,7 @@
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" s="5">
         <v>2</v>
@@ -1996,72 +1996,74 @@
         <v>1</v>
       </c>
       <c r="V13" s="10"/>
-      <c r="W13" s="8"/>
+      <c r="W13" s="8">
+        <v>2</v>
+      </c>
       <c r="X13" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y13" s="10"/>
       <c r="Z13" s="8"/>
       <c r="AA13" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB13" s="10"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AE13" s="10"/>
       <c r="AF13" s="8"/>
       <c r="AG13" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AH13" s="10"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AK13" s="10"/>
       <c r="AL13" s="8"/>
       <c r="AM13" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AN13" s="10"/>
       <c r="AO13" s="8"/>
       <c r="AP13" s="8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="8">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AT13" s="10"/>
       <c r="AU13" s="8"/>
       <c r="AV13" s="8">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AW13" s="10"/>
       <c r="AX13" s="8"/>
       <c r="AY13" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AZ13" s="11">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="BA13" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="2:53" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2711,11 +2713,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2727,6 +2724,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementación del caso de uso cambiar alumno de grupo.
Se implementa el caso de uso cambiar alumno de grupo, se actualizan las platillas y se crean las pruebas de dicha implementación.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2A1EF6-2179-420F-BB1D-77F331D5DB1F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1DBC4ACB-437B-4C13-B655-5C4ED9E7095C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -156,9 +156,6 @@
     <t>Mario</t>
   </si>
   <si>
-    <t>Por iniciar</t>
-  </si>
-  <si>
     <t>Víctor</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>Hecho</t>
+  </si>
+  <si>
+    <t>hecho</t>
   </si>
 </sst>
 </file>
@@ -848,10 +848,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="W12" sqref="W12"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,13 +1139,13 @@
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
       <c r="D6" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="5">
         <v>4</v>
@@ -1254,13 +1254,13 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" s="5">
         <v>2</v>
@@ -1369,13 +1369,13 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="5">
         <v>2</v>
@@ -1484,13 +1484,13 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G9" s="5">
         <v>4</v>
@@ -1599,13 +1599,13 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G10" s="5">
         <v>2</v>
@@ -1720,13 +1720,13 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="5">
         <v>1</v>
@@ -1835,13 +1835,13 @@
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G12" s="5">
         <v>2</v>
@@ -1952,13 +1952,13 @@
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="5">
         <v>3</v>
@@ -2069,13 +2069,13 @@
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="G14" s="5">
         <v>2</v>
@@ -2104,91 +2104,93 @@
         <v>2</v>
       </c>
       <c r="S14" s="10"/>
-      <c r="T14" s="8"/>
+      <c r="T14" s="8">
+        <v>4</v>
+      </c>
       <c r="U14" s="8">
         <f>R14-T14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="V14" s="10"/>
       <c r="W14" s="8"/>
       <c r="X14" s="8">
         <f>U14-W14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="Y14" s="10"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="8">
         <f>X14-Z14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AB14" s="10"/>
       <c r="AC14" s="8"/>
       <c r="AD14" s="8">
         <f>AA14-AC14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AE14" s="10"/>
       <c r="AF14" s="8"/>
       <c r="AG14" s="8">
         <f>AD14-AF14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AH14" s="10"/>
       <c r="AI14" s="8"/>
       <c r="AJ14" s="8">
         <f>AG14-AI14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AK14" s="10"/>
       <c r="AL14" s="8"/>
       <c r="AM14" s="8">
         <f>AJ14-AL14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AN14" s="10"/>
       <c r="AO14" s="8"/>
       <c r="AP14" s="8">
         <f>AM14-AO14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="8"/>
       <c r="AS14" s="8">
         <f>AP14-AR14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AT14" s="10"/>
       <c r="AU14" s="8"/>
       <c r="AV14" s="8">
         <f>AS14-AU14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AW14" s="10"/>
       <c r="AX14" s="8"/>
       <c r="AY14" s="8">
         <f>AV14-AX14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="AZ14" s="11">
         <f>H14+K14+N14+Q14+T14+W14+Z14+AC14+AF14+AI14+AL14+AO14+AR14+AU14+AX14</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BA14" s="11">
         <f>G14-AZ14</f>
-        <v>2</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="15" spans="2:53" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="G15" s="5">
         <v>2</v>
@@ -2714,6 +2716,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2725,11 +2732,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementación del caso de uso cambiar alumno de grupo en el proyecto.
Se agrega el caso de uso cambiar alumno de grupo al flujo del proyecto
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la 5ta Iteración.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1DBC4ACB-437B-4C13-B655-5C4ED9E7095C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E0D5822E-BD97-4154-94DC-E5B67C19D1E1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -848,10 +848,10 @@
   <dimension ref="B1:BA19"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,79 +2105,79 @@
       </c>
       <c r="S14" s="10"/>
       <c r="T14" s="8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U14" s="8">
         <f>R14-T14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="V14" s="10"/>
       <c r="W14" s="8"/>
       <c r="X14" s="8">
         <f>U14-W14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="Y14" s="10"/>
       <c r="Z14" s="8"/>
       <c r="AA14" s="8">
         <f>X14-Z14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AB14" s="10"/>
       <c r="AC14" s="8"/>
       <c r="AD14" s="8">
         <f>AA14-AC14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AE14" s="10"/>
       <c r="AF14" s="8"/>
       <c r="AG14" s="8">
         <f>AD14-AF14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AH14" s="10"/>
       <c r="AI14" s="8"/>
       <c r="AJ14" s="8">
         <f>AG14-AI14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AK14" s="10"/>
       <c r="AL14" s="8"/>
       <c r="AM14" s="8">
         <f>AJ14-AL14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AN14" s="10"/>
       <c r="AO14" s="8"/>
       <c r="AP14" s="8">
         <f>AM14-AO14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="8"/>
       <c r="AS14" s="8">
         <f>AP14-AR14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AT14" s="10"/>
       <c r="AU14" s="8"/>
       <c r="AV14" s="8">
         <f>AS14-AU14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AW14" s="10"/>
       <c r="AX14" s="8"/>
       <c r="AY14" s="8">
         <f>AV14-AX14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AZ14" s="11">
         <f>H14+K14+N14+Q14+T14+W14+Z14+AC14+AF14+AI14+AL14+AO14+AR14+AU14+AX14</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BA14" s="11">
         <f>G14-AZ14</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="15" spans="2:53" x14ac:dyDescent="0.25">
@@ -2716,11 +2716,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2732,6 +2727,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>